<commit_message>
Updated scoring tables and ui
</commit_message>
<xml_diff>
--- a/inst/extdata/Table 4.xlsx
+++ b/inst/extdata/Table 4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SH nomenclature &amp; scoring" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,30 +19,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author>NH</author>
-  </authors>
-  <commentList>
-    <comment ref="F5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Table 1 has a sum score of 60 for MS1 features, how does this map to the value of 50 here?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
@@ -143,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,6 +155,12 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -378,7 +360,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,6 +378,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -622,8 +608,8 @@
   </sheetPr>
   <dimension ref="A2:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S14" activeCellId="0" sqref="S14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -658,19 +644,19 @@
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -700,506 +686,506 @@
       <c r="T4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>42</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="H5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="I5" s="8" t="n">
+        <v>90</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="N5" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="O5" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="P5" s="8" t="n">
         <v>58</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="Q5" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="R5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="K5" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="L5" s="7" t="n">
+      <c r="S5" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="T5" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="M5" s="7" t="n">
-        <v>42</v>
-      </c>
-      <c r="N5" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="O5" s="7" t="n">
-        <v>42</v>
-      </c>
-      <c r="P5" s="7" t="n">
-        <v>70</v>
-      </c>
-      <c r="Q5" s="7" t="n">
-        <v>90</v>
-      </c>
-      <c r="R5" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="S5" s="7" t="n">
-        <v>42</v>
-      </c>
-      <c r="T5" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="U5" s="8" t="n">
+      <c r="U5" s="9" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="C6" s="12" t="n">
         <v>103</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="12" t="n">
         <v>95</v>
       </c>
-      <c r="E6" s="11" t="n">
-        <v>90</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>90</v>
-      </c>
-      <c r="G6" s="11" t="n">
+      <c r="E6" s="12" t="n">
         <v>110</v>
       </c>
-      <c r="H6" s="11" t="n">
+      <c r="F6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>102</v>
+      </c>
+      <c r="H6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="I6" s="12" t="n">
+        <v>171</v>
+      </c>
+      <c r="J6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="K6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="L6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <v>95</v>
+      </c>
+      <c r="N6" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="O6" s="12" t="n">
+        <v>95</v>
+      </c>
+      <c r="P6" s="12" t="n">
         <v>125</v>
       </c>
-      <c r="I6" s="11" t="n">
+      <c r="Q6" s="12" t="n">
         <v>171</v>
       </c>
-      <c r="J6" s="11" t="n">
+      <c r="R6" s="12" t="n">
         <v>110</v>
       </c>
-      <c r="K6" s="11" t="n">
-        <v>125</v>
-      </c>
-      <c r="L6" s="11" t="n">
+      <c r="S6" s="12" t="n">
+        <v>95</v>
+      </c>
+      <c r="T6" s="12" t="n">
         <v>110</v>
       </c>
-      <c r="M6" s="11" t="n">
-        <v>95</v>
-      </c>
-      <c r="N6" s="11" t="n">
-        <v>110</v>
-      </c>
-      <c r="O6" s="11" t="n">
-        <v>95</v>
-      </c>
-      <c r="P6" s="11" t="n">
-        <v>137</v>
-      </c>
-      <c r="Q6" s="11" t="n">
-        <v>171</v>
-      </c>
-      <c r="R6" s="11" t="n">
-        <v>110</v>
-      </c>
-      <c r="S6" s="11" t="n">
-        <v>95</v>
-      </c>
-      <c r="T6" s="11" t="n">
-        <v>110</v>
-      </c>
-      <c r="U6" s="12" t="n">
+      <c r="U6" s="13" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="n">
-        <v>239</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15" t="n">
-        <v>199</v>
-      </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="n">
+        <v>210</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16" t="n">
+        <v>187</v>
+      </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="18" t="n">
+      <c r="B8" s="19" t="n">
         <v>103</v>
       </c>
-      <c r="C8" s="19" t="n">
+      <c r="C8" s="20" t="n">
         <v>103</v>
       </c>
-      <c r="D8" s="19" t="n">
+      <c r="D8" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="20" t="n">
         <v>145</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="F8" s="20" t="n">
         <v>180</v>
       </c>
-      <c r="G8" s="19" t="n">
+      <c r="G8" s="20" t="n">
+        <v>172</v>
+      </c>
+      <c r="H8" s="20" t="n">
         <v>180</v>
       </c>
-      <c r="H8" s="19" t="n">
-        <v>209</v>
-      </c>
-      <c r="I8" s="19" t="n">
+      <c r="I8" s="20" t="n">
         <v>339</v>
       </c>
-      <c r="J8" s="19" t="n">
+      <c r="J8" s="20" t="n">
         <v>145</v>
       </c>
-      <c r="K8" s="19" t="n">
-        <v>209</v>
-      </c>
-      <c r="L8" s="19" t="n">
+      <c r="K8" s="20" t="n">
         <v>180</v>
       </c>
-      <c r="M8" s="19" t="n">
+      <c r="L8" s="20" t="n">
+        <v>180</v>
+      </c>
+      <c r="M8" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="20" t="n">
         <v>145</v>
       </c>
-      <c r="O8" s="19" t="n">
+      <c r="O8" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="P8" s="19" t="n">
-        <v>179</v>
-      </c>
-      <c r="Q8" s="19" t="n">
+      <c r="P8" s="20" t="n">
+        <v>167</v>
+      </c>
+      <c r="Q8" s="20" t="n">
         <v>227</v>
       </c>
-      <c r="R8" s="19" t="n">
+      <c r="R8" s="20" t="n">
         <v>145</v>
       </c>
-      <c r="S8" s="19" t="n">
+      <c r="S8" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="T8" s="19" t="n">
+      <c r="T8" s="20" t="n">
         <v>145</v>
       </c>
-      <c r="U8" s="20" t="n">
+      <c r="U8" s="21" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23" t="n">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="n">
         <v>105</v>
       </c>
-      <c r="E9" s="23" t="n">
+      <c r="E9" s="24" t="n">
         <v>155</v>
       </c>
-      <c r="F9" s="23" t="n">
+      <c r="F9" s="24" t="n">
         <v>190</v>
       </c>
-      <c r="G9" s="23" t="n">
+      <c r="G9" s="24" t="n">
+        <v>182</v>
+      </c>
+      <c r="H9" s="24" t="n">
         <v>190</v>
       </c>
-      <c r="H9" s="23" t="n">
-        <v>219</v>
-      </c>
-      <c r="I9" s="23" t="n">
+      <c r="I9" s="24" t="n">
         <v>349</v>
       </c>
-      <c r="J9" s="23" t="n">
+      <c r="J9" s="24" t="n">
         <v>155</v>
       </c>
-      <c r="K9" s="23" t="n">
-        <v>219</v>
-      </c>
-      <c r="L9" s="23" t="n">
+      <c r="K9" s="24" t="n">
         <v>190</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="24"/>
+      <c r="L9" s="24" t="n">
+        <v>190</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="26" t="n">
+      <c r="B10" s="27" t="n">
         <v>113</v>
       </c>
-      <c r="C10" s="27" t="n">
+      <c r="C10" s="28" t="n">
         <v>113</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="28" t="n">
         <v>115</v>
       </c>
-      <c r="E10" s="27" t="n">
+      <c r="E10" s="28" t="n">
         <v>165</v>
       </c>
-      <c r="F10" s="27" t="n">
+      <c r="F10" s="28" t="n">
         <v>200</v>
       </c>
-      <c r="G10" s="27" t="n">
+      <c r="G10" s="28" t="n">
+        <v>192</v>
+      </c>
+      <c r="H10" s="28" t="n">
         <v>200</v>
       </c>
-      <c r="H10" s="27" t="n">
-        <v>229</v>
-      </c>
-      <c r="I10" s="27" t="n">
+      <c r="I10" s="28" t="n">
         <v>359</v>
       </c>
-      <c r="J10" s="27" t="n">
+      <c r="J10" s="28" t="n">
         <v>165</v>
       </c>
-      <c r="K10" s="27" t="n">
-        <v>229</v>
-      </c>
-      <c r="L10" s="27" t="n">
+      <c r="K10" s="28" t="n">
         <v>200</v>
       </c>
-      <c r="M10" s="27" t="n">
+      <c r="L10" s="28" t="n">
+        <v>200</v>
+      </c>
+      <c r="M10" s="28" t="n">
         <v>105</v>
       </c>
-      <c r="N10" s="27" t="n">
+      <c r="N10" s="28" t="n">
         <v>155</v>
       </c>
-      <c r="O10" s="27" t="n">
+      <c r="O10" s="28" t="n">
         <v>105</v>
       </c>
-      <c r="P10" s="27" t="n">
-        <v>189</v>
-      </c>
-      <c r="Q10" s="27" t="n">
+      <c r="P10" s="28" t="n">
+        <v>177</v>
+      </c>
+      <c r="Q10" s="28" t="n">
         <v>237</v>
       </c>
-      <c r="R10" s="27" t="n">
+      <c r="R10" s="28" t="n">
         <v>155</v>
       </c>
-      <c r="S10" s="27" t="n">
+      <c r="S10" s="28" t="n">
         <v>105</v>
       </c>
-      <c r="T10" s="27" t="n">
+      <c r="T10" s="28" t="n">
         <v>155</v>
       </c>
-      <c r="U10" s="28" t="n">
+      <c r="U10" s="29" t="n">
         <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="n">
+      <c r="B11" s="31"/>
+      <c r="C11" s="32" t="n">
         <v>123</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31" t="n">
-        <v>239</v>
-      </c>
-      <c r="L11" s="31" t="n">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32" t="n">
         <v>210</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31" t="n">
+      <c r="L11" s="32" t="n">
+        <v>210</v>
+      </c>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32" t="n">
         <v>165</v>
       </c>
-      <c r="S11" s="31" t="n">
+      <c r="S11" s="32" t="n">
         <v>115</v>
       </c>
-      <c r="T11" s="31"/>
-      <c r="U11" s="32" t="n">
+      <c r="T11" s="32"/>
+      <c r="U11" s="33" t="n">
         <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="34" t="n">
+      <c r="B12" s="35" t="n">
         <v>123</v>
       </c>
-      <c r="C12" s="35" t="n">
+      <c r="C12" s="36" t="n">
         <v>143</v>
       </c>
-      <c r="D12" s="35" t="n">
+      <c r="D12" s="36" t="n">
         <v>125</v>
       </c>
-      <c r="E12" s="35" t="n">
+      <c r="E12" s="36" t="n">
         <v>175</v>
       </c>
-      <c r="F12" s="35" t="n">
+      <c r="F12" s="36" t="n">
         <v>210</v>
       </c>
-      <c r="G12" s="35" t="n">
-        <v>210</v>
-      </c>
-      <c r="H12" s="35" t="n">
-        <v>249</v>
-      </c>
-      <c r="I12" s="35" t="n">
-        <v>269</v>
-      </c>
-      <c r="J12" s="35" t="n">
+      <c r="G12" s="36" t="n">
+        <v>202</v>
+      </c>
+      <c r="H12" s="36" t="n">
+        <v>220</v>
+      </c>
+      <c r="I12" s="36" t="n">
+        <v>369</v>
+      </c>
+      <c r="J12" s="36" t="n">
         <v>175</v>
       </c>
-      <c r="K12" s="35" t="n">
-        <v>259</v>
-      </c>
-      <c r="L12" s="35" t="n">
+      <c r="K12" s="36" t="n">
         <v>230</v>
       </c>
-      <c r="M12" s="35" t="n">
+      <c r="L12" s="36" t="n">
+        <v>230</v>
+      </c>
+      <c r="M12" s="36" t="n">
         <v>115</v>
       </c>
-      <c r="N12" s="35" t="n">
+      <c r="N12" s="36" t="n">
         <v>165</v>
       </c>
-      <c r="O12" s="35" t="n">
+      <c r="O12" s="36" t="n">
         <v>115</v>
       </c>
-      <c r="P12" s="35" t="n">
-        <v>209</v>
-      </c>
-      <c r="Q12" s="35" t="n">
+      <c r="P12" s="36" t="n">
+        <v>197</v>
+      </c>
+      <c r="Q12" s="36" t="n">
         <v>247</v>
       </c>
-      <c r="R12" s="35" t="n">
+      <c r="R12" s="36" t="n">
         <v>185</v>
       </c>
-      <c r="S12" s="35" t="n">
+      <c r="S12" s="36" t="n">
         <v>135</v>
       </c>
-      <c r="T12" s="35" t="n">
+      <c r="T12" s="36" t="n">
         <v>165</v>
       </c>
-      <c r="U12" s="36" t="n">
+      <c r="U12" s="37" t="n">
         <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="38" t="n">
+      <c r="B13" s="39" t="n">
         <v>133</v>
       </c>
-      <c r="C13" s="39" t="n">
+      <c r="C13" s="40" t="n">
         <v>153</v>
       </c>
-      <c r="D13" s="39" t="n">
+      <c r="D13" s="40" t="n">
         <v>135</v>
       </c>
-      <c r="E13" s="39" t="n">
+      <c r="E13" s="40" t="n">
         <v>185</v>
       </c>
-      <c r="F13" s="39" t="n">
+      <c r="F13" s="40" t="n">
         <v>220</v>
       </c>
-      <c r="G13" s="39" t="n">
-        <v>220</v>
-      </c>
-      <c r="H13" s="39" t="n">
-        <v>259</v>
-      </c>
-      <c r="I13" s="39" t="n">
+      <c r="G13" s="40" t="n">
+        <v>212</v>
+      </c>
+      <c r="H13" s="40" t="n">
+        <v>230</v>
+      </c>
+      <c r="I13" s="40" t="n">
         <v>379</v>
       </c>
-      <c r="J13" s="39" t="n">
+      <c r="J13" s="40" t="n">
         <v>185</v>
       </c>
-      <c r="K13" s="39" t="n">
-        <v>269</v>
-      </c>
-      <c r="L13" s="39" t="n">
+      <c r="K13" s="40" t="n">
         <v>240</v>
       </c>
-      <c r="M13" s="39" t="n">
+      <c r="L13" s="40" t="n">
+        <v>240</v>
+      </c>
+      <c r="M13" s="40" t="n">
         <v>125</v>
       </c>
-      <c r="N13" s="39" t="n">
+      <c r="N13" s="40" t="n">
         <v>175</v>
       </c>
-      <c r="O13" s="39" t="n">
+      <c r="O13" s="40" t="n">
         <v>125</v>
       </c>
-      <c r="P13" s="39" t="n">
-        <v>219</v>
-      </c>
-      <c r="Q13" s="39" t="n">
+      <c r="P13" s="40" t="n">
+        <v>207</v>
+      </c>
+      <c r="Q13" s="40" t="n">
         <v>257</v>
       </c>
-      <c r="R13" s="39" t="n">
+      <c r="R13" s="40" t="n">
         <v>195</v>
       </c>
-      <c r="S13" s="39" t="n">
+      <c r="S13" s="40" t="n">
         <v>145</v>
       </c>
-      <c r="T13" s="39" t="n">
+      <c r="T13" s="40" t="n">
         <v>175</v>
       </c>
-      <c r="U13" s="40" t="n">
+      <c r="U13" s="41" t="n">
         <v>145</v>
       </c>
     </row>
@@ -1211,6 +1197,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>